<commit_message>
⚡ feat(word) Add report
</commit_message>
<xml_diff>
--- a/Diagrams/guides/Diagrama-de-Gantt.xlsx
+++ b/Diagrams/guides/Diagrama-de-Gantt.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\python-webapp\datafactory-migration\Diagrams\guides\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\fisica\datafactory-migration\Diagrams\guides\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C3F561-7A95-44BB-814E-C0C136FDA05C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D256A8-D604-41CF-9E2D-E87C2AC4A8B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="29n/hWAnxvuRyINru/pfsdtCW55KcNepxuwP98WmDqocfLKN9eAhQEKVeiVvCKNzgMBBccplYncdiyrWs3A6aQ==" workbookSaltValue="EN2ks7i2I2hqKnPO9xmdiw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-12555" windowWidth="38640" windowHeight="15720" xr2:uid="{B6FD93E4-D660-4AD6-9289-DE4D1EECF25E}"/>
@@ -65,15 +65,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Cronograma de Actividades</t>
   </si>
   <si>
     <t>Análisis de Impacto.</t>
-  </si>
-  <si>
-    <t>Monitoreo y Optimización.</t>
   </si>
   <si>
     <t>Evaluacion.</t>
@@ -86,9 +83,6 @@
   </si>
   <si>
     <t>Configurar clusters en Databricks.</t>
-  </si>
-  <si>
-    <t>Crea Key Vaults, secretos.</t>
   </si>
   <si>
     <t>Configurar instancia SQL Server.</t>
@@ -119,6 +113,54 @@
   </si>
   <si>
     <t>Configurar CI/CD pipelines.</t>
+  </si>
+  <si>
+    <t>Configurar notebooks en Databricks.</t>
+  </si>
+  <si>
+    <t>Exportar Notebooks de Databricks.</t>
+  </si>
+  <si>
+    <t>Configurar Integration Runtime.</t>
+  </si>
+  <si>
+    <t>Exportar scripts Synapse.</t>
+  </si>
+  <si>
+    <t>Importar tablas en SQL Databases.</t>
+  </si>
+  <si>
+    <t>Exportar backup de  SQL Databases.</t>
+  </si>
+  <si>
+    <t>Crear Key Vaults, secretos.</t>
+  </si>
+  <si>
+    <t>Exportar Logic Apps.</t>
+  </si>
+  <si>
+    <t>importar Logic Apps.</t>
+  </si>
+  <si>
+    <t>Configurar Insights Logic Apps.</t>
+  </si>
+  <si>
+    <t>Importar scripts en Synapse.</t>
+  </si>
+  <si>
+    <t>Configurar Monitor para pipelines ADF.</t>
+  </si>
+  <si>
+    <t>Configurar Storage Services.</t>
+  </si>
+  <si>
+    <t>Exportar contenedores del Storage Account.</t>
+  </si>
+  <si>
+    <t>importar datos en Storage Services.</t>
+  </si>
+  <si>
+    <t>Optimización.</t>
   </si>
 </sst>
 </file>
@@ -224,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="5"/>
@@ -237,9 +279,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -367,9 +406,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.23901110139010401"/>
-          <c:y val="0.29900093352537188"/>
+          <c:y val="0.34139011769760674"/>
           <c:w val="0.73926050354816764"/>
-          <c:h val="0.59242494256635947"/>
+          <c:h val="0.59242504283678266"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -402,46 +441,88 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Gantt!$B$10:$B$22</c:f>
+              <c:f>Gantt!$B$10:$B$36</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>Análisis de Impacto.</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>Configurar Integration Runtime.</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Configurar workspaces en Synapse.</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>Configurar clusters en Databricks.</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>Crea Key Vaults, secretos.</c:v>
-                </c:pt>
                 <c:pt idx="4">
+                  <c:v>Crear Key Vaults, secretos.</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Configurar Storage Services.</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>Configurar instancia SQL Server.</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>Configurar CI/CD pipelines.</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>Exportar pipelines y datasets de ADF.</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>Desplegar pipelines y datasets.</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>Configurar Linked Services.</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
+                  <c:v>Configurar Monitor para pipelines ADF.</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Exportar scripts Synapse.</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Importar scripts en Synapse.</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Exportar Notebooks de Databricks.</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Configurar notebooks en Databricks.</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Exportar contenedores del Storage Account.</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>importar datos en Storage Services.</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Exportar backup de  SQL Databases.</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Importar tablas en SQL Databases.</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>Ejecutar Pipelines.</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="21">
+                  <c:v>Exportar Logic Apps.</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>importar Logic Apps.</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Configurar Insights Logic Apps.</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>Validación.</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>Monitoreo y Optimización.</c:v>
-                </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="25">
+                  <c:v>Optimización.</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>Evaluacion.</c:v>
                 </c:pt>
               </c:strCache>
@@ -449,10 +530,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Gantt!$C$10:$C$22</c:f>
+              <c:f>Gantt!$C$10:$C$36</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>45551</c:v>
                 </c:pt>
@@ -460,7 +541,7 @@
                   <c:v>45558</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45562</c:v>
+                  <c:v>45560</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>45565</c:v>
@@ -475,22 +556,64 @@
                   <c:v>45574</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>45575</c:v>
+                  <c:v>45579</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>45576</c:v>
+                  <c:v>45581</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>45579</c:v>
+                  <c:v>45582</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45581</c:v>
+                  <c:v>45583</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>45586</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>45587</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>45588</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>45590</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>45593</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>45595</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>45596</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>45600</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>45628</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>45630</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>45635</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>45642</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>45644</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>45645</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>45649</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>45650</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -582,46 +705,88 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Gantt!$B$10:$B$22</c:f>
+              <c:f>Gantt!$B$10:$B$36</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>Análisis de Impacto.</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>Configurar Integration Runtime.</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Configurar workspaces en Synapse.</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>Configurar clusters en Databricks.</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>Crea Key Vaults, secretos.</c:v>
-                </c:pt>
                 <c:pt idx="4">
+                  <c:v>Crear Key Vaults, secretos.</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Configurar Storage Services.</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>Configurar instancia SQL Server.</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>Configurar CI/CD pipelines.</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>Exportar pipelines y datasets de ADF.</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>Desplegar pipelines y datasets.</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>Configurar Linked Services.</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
+                  <c:v>Configurar Monitor para pipelines ADF.</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Exportar scripts Synapse.</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Importar scripts en Synapse.</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Exportar Notebooks de Databricks.</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Configurar notebooks en Databricks.</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Exportar contenedores del Storage Account.</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>importar datos en Storage Services.</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Exportar backup de  SQL Databases.</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Importar tablas en SQL Databases.</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>Ejecutar Pipelines.</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="21">
+                  <c:v>Exportar Logic Apps.</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>importar Logic Apps.</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Configurar Insights Logic Apps.</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>Validación.</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>Monitoreo y Optimización.</c:v>
-                </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="25">
+                  <c:v>Optimización.</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>Evaluacion.</c:v>
                 </c:pt>
               </c:strCache>
@@ -629,18 +794,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Gantt!$D$10:$D$22</c:f>
+              <c:f>Gantt!$D$10:$D$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2</c:v>
@@ -652,24 +817,66 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -749,7 +956,7 @@
         <c:axId val="1184412656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="45593"/>
+          <c:max val="45657"/>
           <c:min val="45551"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -813,6 +1020,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.41818479185210661"/>
+          <c:y val="0.94617187205666287"/>
+          <c:w val="0.16363041629578678"/>
+          <c:h val="3.4689371962475977E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1727,8 +1944,8 @@
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>428624</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3083,49 +3300,49 @@
   <sheetPr>
     <tabColor theme="8" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="B6:F27"/>
+  <dimension ref="B6:F41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y23" sqref="Y23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.42578125" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3"/>
-      <c r="C9" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="9" t="s">
+      <c r="C9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>16</v>
       </c>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="2:6" ht="22.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="11" t="s">
+    <row r="10" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="7">
         <v>45551</v>
       </c>
       <c r="D10" s="5">
@@ -3136,212 +3353,436 @@
         <v>45558</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="12" t="s">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="7">
+        <f>$E10</f>
+        <v>45558</v>
+      </c>
+      <c r="D11" s="5">
+        <v>2</v>
+      </c>
+      <c r="E11" s="4">
+        <f>$C11+$D11</f>
+        <v>45560</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="7">
+        <f t="shared" ref="C12:C36" si="0">$E11</f>
+        <v>45560</v>
+      </c>
+      <c r="D12" s="6">
         <v>5</v>
       </c>
-      <c r="C11" s="8">
-        <f>E10</f>
-        <v>45558</v>
-      </c>
-      <c r="D11" s="7">
-        <v>4</v>
-      </c>
-      <c r="E11" s="6">
-        <f>C11+D11</f>
-        <v>45562</v>
+      <c r="E12" s="4">
+        <f t="shared" ref="E12:E36" si="1">$C12+$D12</f>
+        <v>45565</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="8">
-        <f t="shared" ref="C12:C22" si="0">E11</f>
-        <v>45562</v>
-      </c>
-      <c r="D12" s="7">
-        <v>3</v>
-      </c>
-      <c r="E12" s="6">
-        <f>C12+D12</f>
-        <v>45565</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="8">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="7">
         <f t="shared" si="0"/>
         <v>45565</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="6">
         <v>2</v>
       </c>
-      <c r="E13" s="6">
-        <f t="shared" ref="E13:E22" si="1">C13+D13</f>
+      <c r="E13" s="4">
+        <f t="shared" si="1"/>
         <v>45567</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="8">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="7">
         <f t="shared" si="0"/>
         <v>45567</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="6">
         <v>5</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="4">
         <f t="shared" si="1"/>
         <v>45572</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="8">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="7">
         <f t="shared" si="0"/>
         <v>45572</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="6">
         <v>2</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="4">
         <f t="shared" si="1"/>
         <v>45574</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="8">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="7">
         <f t="shared" si="0"/>
         <v>45574</v>
       </c>
-      <c r="D16" s="7">
-        <v>1</v>
-      </c>
-      <c r="E16" s="6">
-        <f t="shared" si="1"/>
-        <v>45575</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="8">
-        <f t="shared" si="0"/>
-        <v>45575</v>
-      </c>
-      <c r="D17" s="7">
-        <v>1</v>
-      </c>
-      <c r="E17" s="6">
-        <f t="shared" si="1"/>
-        <v>45576</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="8">
-        <f t="shared" si="0"/>
-        <v>45576</v>
-      </c>
-      <c r="D18" s="7">
-        <v>3</v>
-      </c>
-      <c r="E18" s="6">
+      <c r="D16" s="6">
+        <v>5</v>
+      </c>
+      <c r="E16" s="4">
         <f t="shared" si="1"/>
         <v>45579</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="8">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="7">
         <f t="shared" si="0"/>
         <v>45579</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D17" s="6">
         <v>2</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E17" s="4">
         <f t="shared" si="1"/>
         <v>45581</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="8">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="7">
         <f t="shared" si="0"/>
         <v>45581</v>
       </c>
-      <c r="D20" s="7">
-        <v>5</v>
-      </c>
-      <c r="E20" s="6">
+      <c r="D18" s="6">
+        <v>1</v>
+      </c>
+      <c r="E18" s="4">
+        <f t="shared" si="1"/>
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="7">
+        <f t="shared" si="0"/>
+        <v>45582</v>
+      </c>
+      <c r="D19" s="6">
+        <v>1</v>
+      </c>
+      <c r="E19" s="4">
+        <f t="shared" si="1"/>
+        <v>45583</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="7">
+        <f t="shared" si="0"/>
+        <v>45583</v>
+      </c>
+      <c r="D20" s="6">
+        <v>3</v>
+      </c>
+      <c r="E20" s="4">
         <f t="shared" si="1"/>
         <v>45586</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C21" s="8">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="7">
         <f t="shared" si="0"/>
         <v>45586</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="6">
         <v>1</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="4">
         <f t="shared" si="1"/>
         <v>45587</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="8">
+      <c r="B22" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="7">
         <f t="shared" si="0"/>
         <v>45587</v>
       </c>
-      <c r="D22" s="7">
-        <v>6</v>
-      </c>
-      <c r="E22" s="6">
+      <c r="D22" s="6">
+        <v>1</v>
+      </c>
+      <c r="E22" s="4">
+        <f t="shared" si="1"/>
+        <v>45588</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="7">
+        <f t="shared" si="0"/>
+        <v>45588</v>
+      </c>
+      <c r="D23" s="6">
+        <v>2</v>
+      </c>
+      <c r="E23" s="4">
+        <f t="shared" si="1"/>
+        <v>45590</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="7">
+        <f t="shared" si="0"/>
+        <v>45590</v>
+      </c>
+      <c r="D24" s="6">
+        <v>3</v>
+      </c>
+      <c r="E24" s="4">
         <f t="shared" si="1"/>
         <v>45593</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24"/>
-    </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25"/>
+      <c r="B25" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="7">
+        <f t="shared" si="0"/>
+        <v>45593</v>
+      </c>
+      <c r="D25" s="6">
+        <v>2</v>
+      </c>
+      <c r="E25" s="4">
+        <f t="shared" si="1"/>
+        <v>45595</v>
+      </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26"/>
+      <c r="B26" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="7">
+        <f t="shared" si="0"/>
+        <v>45595</v>
+      </c>
+      <c r="D26" s="6">
+        <v>1</v>
+      </c>
+      <c r="E26" s="4">
+        <f t="shared" si="1"/>
+        <v>45596</v>
+      </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27"/>
+      <c r="B27" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="7">
+        <f t="shared" si="0"/>
+        <v>45596</v>
+      </c>
+      <c r="D27" s="6">
+        <v>4</v>
+      </c>
+      <c r="E27" s="4">
+        <f t="shared" si="1"/>
+        <v>45600</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="7">
+        <f t="shared" si="0"/>
+        <v>45600</v>
+      </c>
+      <c r="D28" s="6">
+        <v>28</v>
+      </c>
+      <c r="E28" s="4">
+        <f t="shared" si="1"/>
+        <v>45628</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="7">
+        <f t="shared" si="0"/>
+        <v>45628</v>
+      </c>
+      <c r="D29" s="6">
+        <v>2</v>
+      </c>
+      <c r="E29" s="4">
+        <f t="shared" si="1"/>
+        <v>45630</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="7">
+        <f t="shared" si="0"/>
+        <v>45630</v>
+      </c>
+      <c r="D30" s="6">
+        <v>5</v>
+      </c>
+      <c r="E30" s="4">
+        <f t="shared" si="1"/>
+        <v>45635</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="7">
+        <f t="shared" si="0"/>
+        <v>45635</v>
+      </c>
+      <c r="D31" s="6">
+        <v>7</v>
+      </c>
+      <c r="E31" s="4">
+        <f t="shared" si="1"/>
+        <v>45642</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="7">
+        <f t="shared" si="0"/>
+        <v>45642</v>
+      </c>
+      <c r="D32" s="6">
+        <v>2</v>
+      </c>
+      <c r="E32" s="4">
+        <f t="shared" si="1"/>
+        <v>45644</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="7">
+        <f t="shared" si="0"/>
+        <v>45644</v>
+      </c>
+      <c r="D33" s="6">
+        <v>1</v>
+      </c>
+      <c r="E33" s="4">
+        <f t="shared" si="1"/>
+        <v>45645</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="7">
+        <f t="shared" si="0"/>
+        <v>45645</v>
+      </c>
+      <c r="D34" s="6">
+        <v>4</v>
+      </c>
+      <c r="E34" s="4">
+        <f t="shared" si="1"/>
+        <v>45649</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="7">
+        <f t="shared" si="0"/>
+        <v>45649</v>
+      </c>
+      <c r="D35" s="6">
+        <v>1</v>
+      </c>
+      <c r="E35" s="4">
+        <f t="shared" si="1"/>
+        <v>45650</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="7">
+        <f t="shared" si="0"/>
+        <v>45650</v>
+      </c>
+      <c r="D36" s="6">
+        <v>6</v>
+      </c>
+      <c r="E36" s="4">
+        <f t="shared" si="1"/>
+        <v>45656</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
🔀  feat(word) Add report (#8)
</commit_message>
<xml_diff>
--- a/Diagrams/guides/Diagrama-de-Gantt.xlsx
+++ b/Diagrams/guides/Diagrama-de-Gantt.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\python-webapp\datafactory-migration\Diagrams\guides\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\fisica\datafactory-migration\Diagrams\guides\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C3F561-7A95-44BB-814E-C0C136FDA05C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D256A8-D604-41CF-9E2D-E87C2AC4A8B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="29n/hWAnxvuRyINru/pfsdtCW55KcNepxuwP98WmDqocfLKN9eAhQEKVeiVvCKNzgMBBccplYncdiyrWs3A6aQ==" workbookSaltValue="EN2ks7i2I2hqKnPO9xmdiw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-12555" windowWidth="38640" windowHeight="15720" xr2:uid="{B6FD93E4-D660-4AD6-9289-DE4D1EECF25E}"/>
@@ -65,15 +65,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Cronograma de Actividades</t>
   </si>
   <si>
     <t>Análisis de Impacto.</t>
-  </si>
-  <si>
-    <t>Monitoreo y Optimización.</t>
   </si>
   <si>
     <t>Evaluacion.</t>
@@ -86,9 +83,6 @@
   </si>
   <si>
     <t>Configurar clusters en Databricks.</t>
-  </si>
-  <si>
-    <t>Crea Key Vaults, secretos.</t>
   </si>
   <si>
     <t>Configurar instancia SQL Server.</t>
@@ -119,6 +113,54 @@
   </si>
   <si>
     <t>Configurar CI/CD pipelines.</t>
+  </si>
+  <si>
+    <t>Configurar notebooks en Databricks.</t>
+  </si>
+  <si>
+    <t>Exportar Notebooks de Databricks.</t>
+  </si>
+  <si>
+    <t>Configurar Integration Runtime.</t>
+  </si>
+  <si>
+    <t>Exportar scripts Synapse.</t>
+  </si>
+  <si>
+    <t>Importar tablas en SQL Databases.</t>
+  </si>
+  <si>
+    <t>Exportar backup de  SQL Databases.</t>
+  </si>
+  <si>
+    <t>Crear Key Vaults, secretos.</t>
+  </si>
+  <si>
+    <t>Exportar Logic Apps.</t>
+  </si>
+  <si>
+    <t>importar Logic Apps.</t>
+  </si>
+  <si>
+    <t>Configurar Insights Logic Apps.</t>
+  </si>
+  <si>
+    <t>Importar scripts en Synapse.</t>
+  </si>
+  <si>
+    <t>Configurar Monitor para pipelines ADF.</t>
+  </si>
+  <si>
+    <t>Configurar Storage Services.</t>
+  </si>
+  <si>
+    <t>Exportar contenedores del Storage Account.</t>
+  </si>
+  <si>
+    <t>importar datos en Storage Services.</t>
+  </si>
+  <si>
+    <t>Optimización.</t>
   </si>
 </sst>
 </file>
@@ -224,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="5"/>
@@ -237,9 +279,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -367,9 +406,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.23901110139010401"/>
-          <c:y val="0.29900093352537188"/>
+          <c:y val="0.34139011769760674"/>
           <c:w val="0.73926050354816764"/>
-          <c:h val="0.59242494256635947"/>
+          <c:h val="0.59242504283678266"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -402,46 +441,88 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Gantt!$B$10:$B$22</c:f>
+              <c:f>Gantt!$B$10:$B$36</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>Análisis de Impacto.</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>Configurar Integration Runtime.</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Configurar workspaces en Synapse.</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>Configurar clusters en Databricks.</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>Crea Key Vaults, secretos.</c:v>
-                </c:pt>
                 <c:pt idx="4">
+                  <c:v>Crear Key Vaults, secretos.</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Configurar Storage Services.</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>Configurar instancia SQL Server.</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>Configurar CI/CD pipelines.</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>Exportar pipelines y datasets de ADF.</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>Desplegar pipelines y datasets.</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>Configurar Linked Services.</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
+                  <c:v>Configurar Monitor para pipelines ADF.</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Exportar scripts Synapse.</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Importar scripts en Synapse.</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Exportar Notebooks de Databricks.</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Configurar notebooks en Databricks.</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Exportar contenedores del Storage Account.</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>importar datos en Storage Services.</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Exportar backup de  SQL Databases.</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Importar tablas en SQL Databases.</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>Ejecutar Pipelines.</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="21">
+                  <c:v>Exportar Logic Apps.</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>importar Logic Apps.</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Configurar Insights Logic Apps.</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>Validación.</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>Monitoreo y Optimización.</c:v>
-                </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="25">
+                  <c:v>Optimización.</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>Evaluacion.</c:v>
                 </c:pt>
               </c:strCache>
@@ -449,10 +530,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Gantt!$C$10:$C$22</c:f>
+              <c:f>Gantt!$C$10:$C$36</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>45551</c:v>
                 </c:pt>
@@ -460,7 +541,7 @@
                   <c:v>45558</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45562</c:v>
+                  <c:v>45560</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>45565</c:v>
@@ -475,22 +556,64 @@
                   <c:v>45574</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>45575</c:v>
+                  <c:v>45579</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>45576</c:v>
+                  <c:v>45581</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>45579</c:v>
+                  <c:v>45582</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45581</c:v>
+                  <c:v>45583</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>45586</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>45587</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>45588</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>45590</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>45593</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>45595</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>45596</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>45600</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>45628</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>45630</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>45635</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>45642</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>45644</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>45645</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>45649</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>45650</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -582,46 +705,88 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Gantt!$B$10:$B$22</c:f>
+              <c:f>Gantt!$B$10:$B$36</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>Análisis de Impacto.</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>Configurar Integration Runtime.</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Configurar workspaces en Synapse.</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>Configurar clusters en Databricks.</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>Crea Key Vaults, secretos.</c:v>
-                </c:pt>
                 <c:pt idx="4">
+                  <c:v>Crear Key Vaults, secretos.</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Configurar Storage Services.</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>Configurar instancia SQL Server.</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>Configurar CI/CD pipelines.</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>Exportar pipelines y datasets de ADF.</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>Desplegar pipelines y datasets.</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>Configurar Linked Services.</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
+                  <c:v>Configurar Monitor para pipelines ADF.</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Exportar scripts Synapse.</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Importar scripts en Synapse.</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Exportar Notebooks de Databricks.</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Configurar notebooks en Databricks.</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Exportar contenedores del Storage Account.</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>importar datos en Storage Services.</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Exportar backup de  SQL Databases.</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Importar tablas en SQL Databases.</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>Ejecutar Pipelines.</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="21">
+                  <c:v>Exportar Logic Apps.</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>importar Logic Apps.</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Configurar Insights Logic Apps.</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>Validación.</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>Monitoreo y Optimización.</c:v>
-                </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="25">
+                  <c:v>Optimización.</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>Evaluacion.</c:v>
                 </c:pt>
               </c:strCache>
@@ -629,18 +794,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Gantt!$D$10:$D$22</c:f>
+              <c:f>Gantt!$D$10:$D$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2</c:v>
@@ -652,24 +817,66 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -749,7 +956,7 @@
         <c:axId val="1184412656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="45593"/>
+          <c:max val="45657"/>
           <c:min val="45551"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -813,6 +1020,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.41818479185210661"/>
+          <c:y val="0.94617187205666287"/>
+          <c:w val="0.16363041629578678"/>
+          <c:h val="3.4689371962475977E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1727,8 +1944,8 @@
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>428624</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3083,49 +3300,49 @@
   <sheetPr>
     <tabColor theme="8" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="B6:F27"/>
+  <dimension ref="B6:F41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y23" sqref="Y23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.42578125" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3"/>
-      <c r="C9" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="9" t="s">
+      <c r="C9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>16</v>
       </c>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="2:6" ht="22.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="11" t="s">
+    <row r="10" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="7">
         <v>45551</v>
       </c>
       <c r="D10" s="5">
@@ -3136,212 +3353,436 @@
         <v>45558</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="12" t="s">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="7">
+        <f>$E10</f>
+        <v>45558</v>
+      </c>
+      <c r="D11" s="5">
+        <v>2</v>
+      </c>
+      <c r="E11" s="4">
+        <f>$C11+$D11</f>
+        <v>45560</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="7">
+        <f t="shared" ref="C12:C36" si="0">$E11</f>
+        <v>45560</v>
+      </c>
+      <c r="D12" s="6">
         <v>5</v>
       </c>
-      <c r="C11" s="8">
-        <f>E10</f>
-        <v>45558</v>
-      </c>
-      <c r="D11" s="7">
-        <v>4</v>
-      </c>
-      <c r="E11" s="6">
-        <f>C11+D11</f>
-        <v>45562</v>
+      <c r="E12" s="4">
+        <f t="shared" ref="E12:E36" si="1">$C12+$D12</f>
+        <v>45565</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="8">
-        <f t="shared" ref="C12:C22" si="0">E11</f>
-        <v>45562</v>
-      </c>
-      <c r="D12" s="7">
-        <v>3</v>
-      </c>
-      <c r="E12" s="6">
-        <f>C12+D12</f>
-        <v>45565</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="8">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="7">
         <f t="shared" si="0"/>
         <v>45565</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="6">
         <v>2</v>
       </c>
-      <c r="E13" s="6">
-        <f t="shared" ref="E13:E22" si="1">C13+D13</f>
+      <c r="E13" s="4">
+        <f t="shared" si="1"/>
         <v>45567</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="8">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="7">
         <f t="shared" si="0"/>
         <v>45567</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="6">
         <v>5</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="4">
         <f t="shared" si="1"/>
         <v>45572</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="8">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="7">
         <f t="shared" si="0"/>
         <v>45572</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="6">
         <v>2</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="4">
         <f t="shared" si="1"/>
         <v>45574</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="8">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="7">
         <f t="shared" si="0"/>
         <v>45574</v>
       </c>
-      <c r="D16" s="7">
-        <v>1</v>
-      </c>
-      <c r="E16" s="6">
-        <f t="shared" si="1"/>
-        <v>45575</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="8">
-        <f t="shared" si="0"/>
-        <v>45575</v>
-      </c>
-      <c r="D17" s="7">
-        <v>1</v>
-      </c>
-      <c r="E17" s="6">
-        <f t="shared" si="1"/>
-        <v>45576</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="8">
-        <f t="shared" si="0"/>
-        <v>45576</v>
-      </c>
-      <c r="D18" s="7">
-        <v>3</v>
-      </c>
-      <c r="E18" s="6">
+      <c r="D16" s="6">
+        <v>5</v>
+      </c>
+      <c r="E16" s="4">
         <f t="shared" si="1"/>
         <v>45579</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="8">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="7">
         <f t="shared" si="0"/>
         <v>45579</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D17" s="6">
         <v>2</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E17" s="4">
         <f t="shared" si="1"/>
         <v>45581</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="8">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="7">
         <f t="shared" si="0"/>
         <v>45581</v>
       </c>
-      <c r="D20" s="7">
-        <v>5</v>
-      </c>
-      <c r="E20" s="6">
+      <c r="D18" s="6">
+        <v>1</v>
+      </c>
+      <c r="E18" s="4">
+        <f t="shared" si="1"/>
+        <v>45582</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="7">
+        <f t="shared" si="0"/>
+        <v>45582</v>
+      </c>
+      <c r="D19" s="6">
+        <v>1</v>
+      </c>
+      <c r="E19" s="4">
+        <f t="shared" si="1"/>
+        <v>45583</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="7">
+        <f t="shared" si="0"/>
+        <v>45583</v>
+      </c>
+      <c r="D20" s="6">
+        <v>3</v>
+      </c>
+      <c r="E20" s="4">
         <f t="shared" si="1"/>
         <v>45586</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C21" s="8">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="7">
         <f t="shared" si="0"/>
         <v>45586</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="6">
         <v>1</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="4">
         <f t="shared" si="1"/>
         <v>45587</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="8">
+      <c r="B22" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="7">
         <f t="shared" si="0"/>
         <v>45587</v>
       </c>
-      <c r="D22" s="7">
-        <v>6</v>
-      </c>
-      <c r="E22" s="6">
+      <c r="D22" s="6">
+        <v>1</v>
+      </c>
+      <c r="E22" s="4">
+        <f t="shared" si="1"/>
+        <v>45588</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="7">
+        <f t="shared" si="0"/>
+        <v>45588</v>
+      </c>
+      <c r="D23" s="6">
+        <v>2</v>
+      </c>
+      <c r="E23" s="4">
+        <f t="shared" si="1"/>
+        <v>45590</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="7">
+        <f t="shared" si="0"/>
+        <v>45590</v>
+      </c>
+      <c r="D24" s="6">
+        <v>3</v>
+      </c>
+      <c r="E24" s="4">
         <f t="shared" si="1"/>
         <v>45593</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24"/>
-    </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25"/>
+      <c r="B25" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="7">
+        <f t="shared" si="0"/>
+        <v>45593</v>
+      </c>
+      <c r="D25" s="6">
+        <v>2</v>
+      </c>
+      <c r="E25" s="4">
+        <f t="shared" si="1"/>
+        <v>45595</v>
+      </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26"/>
+      <c r="B26" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="7">
+        <f t="shared" si="0"/>
+        <v>45595</v>
+      </c>
+      <c r="D26" s="6">
+        <v>1</v>
+      </c>
+      <c r="E26" s="4">
+        <f t="shared" si="1"/>
+        <v>45596</v>
+      </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27"/>
+      <c r="B27" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="7">
+        <f t="shared" si="0"/>
+        <v>45596</v>
+      </c>
+      <c r="D27" s="6">
+        <v>4</v>
+      </c>
+      <c r="E27" s="4">
+        <f t="shared" si="1"/>
+        <v>45600</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="7">
+        <f t="shared" si="0"/>
+        <v>45600</v>
+      </c>
+      <c r="D28" s="6">
+        <v>28</v>
+      </c>
+      <c r="E28" s="4">
+        <f t="shared" si="1"/>
+        <v>45628</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="7">
+        <f t="shared" si="0"/>
+        <v>45628</v>
+      </c>
+      <c r="D29" s="6">
+        <v>2</v>
+      </c>
+      <c r="E29" s="4">
+        <f t="shared" si="1"/>
+        <v>45630</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="7">
+        <f t="shared" si="0"/>
+        <v>45630</v>
+      </c>
+      <c r="D30" s="6">
+        <v>5</v>
+      </c>
+      <c r="E30" s="4">
+        <f t="shared" si="1"/>
+        <v>45635</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="7">
+        <f t="shared" si="0"/>
+        <v>45635</v>
+      </c>
+      <c r="D31" s="6">
+        <v>7</v>
+      </c>
+      <c r="E31" s="4">
+        <f t="shared" si="1"/>
+        <v>45642</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="7">
+        <f t="shared" si="0"/>
+        <v>45642</v>
+      </c>
+      <c r="D32" s="6">
+        <v>2</v>
+      </c>
+      <c r="E32" s="4">
+        <f t="shared" si="1"/>
+        <v>45644</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="7">
+        <f t="shared" si="0"/>
+        <v>45644</v>
+      </c>
+      <c r="D33" s="6">
+        <v>1</v>
+      </c>
+      <c r="E33" s="4">
+        <f t="shared" si="1"/>
+        <v>45645</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="7">
+        <f t="shared" si="0"/>
+        <v>45645</v>
+      </c>
+      <c r="D34" s="6">
+        <v>4</v>
+      </c>
+      <c r="E34" s="4">
+        <f t="shared" si="1"/>
+        <v>45649</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="7">
+        <f t="shared" si="0"/>
+        <v>45649</v>
+      </c>
+      <c r="D35" s="6">
+        <v>1</v>
+      </c>
+      <c r="E35" s="4">
+        <f t="shared" si="1"/>
+        <v>45650</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="7">
+        <f t="shared" si="0"/>
+        <v>45650</v>
+      </c>
+      <c r="D36" s="6">
+        <v>6</v>
+      </c>
+      <c r="E36" s="4">
+        <f t="shared" si="1"/>
+        <v>45656</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
⚡ feat(powerpoint) Change diagram
</commit_message>
<xml_diff>
--- a/Diagrams/guides/Diagrama-de-Gantt.xlsx
+++ b/Diagrams/guides/Diagrama-de-Gantt.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\fisica\datafactory-migration\Diagrams\guides\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\soap-iis\datafactory-migration\Diagrams\guides\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D256A8-D604-41CF-9E2D-E87C2AC4A8B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B61AEE7B-FBCC-40A3-A85E-4633E735A3C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="29n/hWAnxvuRyINru/pfsdtCW55KcNepxuwP98WmDqocfLKN9eAhQEKVeiVvCKNzgMBBccplYncdiyrWs3A6aQ==" workbookSaltValue="EN2ks7i2I2hqKnPO9xmdiw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-12555" windowWidth="38640" windowHeight="15720" xr2:uid="{B6FD93E4-D660-4AD6-9289-DE4D1EECF25E}"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Cronograma de Actividades</t>
   </si>
@@ -161,6 +161,9 @@
   </si>
   <si>
     <t>Optimización.</t>
+  </si>
+  <si>
+    <t>Ejecutar tests.</t>
   </si>
 </sst>
 </file>
@@ -355,7 +358,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="es-CO" b="1" baseline="0"/>
-              <a:t> migracion.</a:t>
+              <a:t> migración.</a:t>
             </a:r>
             <a:endParaRPr lang="es-CO" b="1"/>
           </a:p>
@@ -365,8 +368,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.44586351021263132"/>
-          <c:y val="4.1666677182181804E-2"/>
+          <c:x val="0.4472062915163405"/>
+          <c:y val="1.5860299720599443E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -406,9 +409,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.23901110139010401"/>
-          <c:y val="0.34139011769760674"/>
+          <c:y val="0.1819698352923276"/>
           <c:w val="0.73926050354816764"/>
-          <c:h val="0.59242504283678266"/>
+          <c:h val="0.75184525847312567"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -441,9 +444,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Gantt!$B$10:$B$36</c:f>
+              <c:f>Gantt!$B$10:$B$37</c:f>
               <c:strCache>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>Análisis de Impacto.</c:v>
                 </c:pt>
@@ -508,21 +511,24 @@
                   <c:v>Ejecutar Pipelines.</c:v>
                 </c:pt>
                 <c:pt idx="21">
+                  <c:v>Ejecutar tests.</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>Exportar Logic Apps.</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>importar Logic Apps.</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>Configurar Insights Logic Apps.</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>Validación.</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>Optimización.</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>Evaluacion.</c:v>
                 </c:pt>
               </c:strCache>
@@ -530,10 +536,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Gantt!$C$10:$C$36</c:f>
+              <c:f>Gantt!$C$10:$C$37</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>45551</c:v>
                 </c:pt>
@@ -601,19 +607,22 @@
                   <c:v>45635</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>45642</c:v>
+                  <c:v>45636</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>45644</c:v>
+                  <c:v>45649</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>45645</c:v>
+                  <c:v>45651</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>45649</c:v>
+                  <c:v>45652</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>45650</c:v>
+                  <c:v>45656</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>45657</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -705,9 +714,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Gantt!$B$10:$B$36</c:f>
+              <c:f>Gantt!$B$10:$B$37</c:f>
               <c:strCache>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>Análisis de Impacto.</c:v>
                 </c:pt>
@@ -772,21 +781,24 @@
                   <c:v>Ejecutar Pipelines.</c:v>
                 </c:pt>
                 <c:pt idx="21">
+                  <c:v>Ejecutar tests.</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>Exportar Logic Apps.</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>importar Logic Apps.</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>Configurar Insights Logic Apps.</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>Validación.</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>Optimización.</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>Evaluacion.</c:v>
                 </c:pt>
               </c:strCache>
@@ -794,10 +806,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Gantt!$D$10:$D$36</c:f>
+              <c:f>Gantt!$D$10:$D$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>7</c:v>
                 </c:pt>
@@ -862,21 +874,24 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>7</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="22">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -956,7 +971,7 @@
         <c:axId val="1184412656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="45657"/>
+          <c:max val="45663"/>
           <c:min val="45551"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1936,16 +1951,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>114301</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>428624</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3300,10 +3315,10 @@
   <sheetPr>
     <tabColor theme="8" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="B6:F41"/>
+  <dimension ref="B6:F42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="X27" sqref="X27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3374,14 +3389,14 @@
         <v>4</v>
       </c>
       <c r="C12" s="7">
-        <f t="shared" ref="C12:C36" si="0">$E11</f>
+        <f t="shared" ref="C12:C37" si="0">$E11</f>
         <v>45560</v>
       </c>
       <c r="D12" s="6">
         <v>5</v>
       </c>
       <c r="E12" s="4">
-        <f t="shared" ref="E12:E36" si="1">$C12+$D12</f>
+        <f t="shared" ref="E12:E37" si="1">$C12+$D12</f>
         <v>45565</v>
       </c>
     </row>
@@ -3675,102 +3690,115 @@
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="11" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C31" s="7">
         <f t="shared" si="0"/>
         <v>45635</v>
       </c>
       <c r="D31" s="6">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E31" s="4">
         <f t="shared" si="1"/>
-        <v>45642</v>
+        <v>45636</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C32" s="7">
         <f t="shared" si="0"/>
-        <v>45642</v>
+        <v>45636</v>
       </c>
       <c r="D32" s="6">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E32" s="4">
         <f t="shared" si="1"/>
-        <v>45644</v>
+        <v>45649</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C33" s="7">
         <f t="shared" si="0"/>
-        <v>45644</v>
+        <v>45649</v>
       </c>
       <c r="D33" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E33" s="4">
         <f t="shared" si="1"/>
-        <v>45645</v>
+        <v>45651</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="11" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C34" s="7">
         <f t="shared" si="0"/>
-        <v>45645</v>
+        <v>45651</v>
       </c>
       <c r="D34" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E34" s="4">
         <f t="shared" si="1"/>
-        <v>45649</v>
+        <v>45652</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="11" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="C35" s="7">
         <f t="shared" si="0"/>
-        <v>45649</v>
+        <v>45652</v>
       </c>
       <c r="D35" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E35" s="4">
         <f t="shared" si="1"/>
-        <v>45650</v>
+        <v>45656</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="11" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="C36" s="7">
         <f t="shared" si="0"/>
-        <v>45650</v>
+        <v>45656</v>
       </c>
       <c r="D36" s="6">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E36" s="4">
         <f t="shared" si="1"/>
-        <v>45656</v>
+        <v>45657</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37"/>
+      <c r="B37" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="7">
+        <f t="shared" si="0"/>
+        <v>45657</v>
+      </c>
+      <c r="D37" s="6">
+        <v>6</v>
+      </c>
+      <c r="E37" s="4">
+        <f t="shared" si="1"/>
+        <v>45663</v>
+      </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38"/>
@@ -3783,6 +3811,9 @@
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41"/>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B42"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>